<commit_message>
added 241018 ragas evaluation result and updated history
</commit_message>
<xml_diff>
--- a/chatgpt_performance_metric/Evaluation_Release_Result/Evaluation_Release_History.xlsx
+++ b/chatgpt_performance_metric/Evaluation_Release_Result/Evaluation_Release_History.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\tom\python_project\perf_metric_ing\perf_metric\chatgpt_performance_metric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\project\AI_Application\rag\source\ragas_evaluation\perf_metric\chatgpt_performance_metric\evaluation_release_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFB81D2-308B-4F66-99B3-AC047B2DBB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A46EBAB-E4FD-4454-B7CC-95DBB792A9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85E0B42A-1E2E-4653-9973-9AFC057EC341}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85E0B42A-1E2E-4653-9973-9AFC057EC341}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Release_History" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="16">
   <si>
     <t>challenger.txt</t>
   </si>
@@ -111,14 +111,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -138,7 +138,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,7 +212,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -235,6 +241,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,21 +586,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D663431-DE91-43EB-971D-8A92CF748157}">
-  <dimension ref="D3:J12"/>
+  <dimension ref="D3:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="57.44140625" style="1" customWidth="1"/>
-    <col min="5" max="133" width="15.77734375" style="1" customWidth="1"/>
-    <col min="134" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="3" width="8.8984375" style="1"/>
+    <col min="4" max="4" width="57.3984375" style="1" customWidth="1"/>
+    <col min="5" max="133" width="15.796875" style="1" customWidth="1"/>
+    <col min="134" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:10" ht="17.399999999999999">
+    <row r="3" spans="4:13" ht="17.399999999999999">
       <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
@@ -599,8 +614,13 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
+      <c r="K3" s="10">
+        <v>45583</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="4:10" ht="104.4">
+    <row r="4" spans="4:13" ht="87">
       <c r="D4" s="9"/>
       <c r="E4" s="3" t="s">
         <v>8</v>
@@ -620,8 +640,17 @@
       <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="K4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="4:10" ht="17.399999999999999">
+    <row r="5" spans="4:13" ht="17.399999999999999">
       <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
@@ -643,8 +672,17 @@
       <c r="J5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="4:10" ht="17.399999999999999">
+    <row r="6" spans="4:13" ht="17.399999999999999">
       <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
@@ -666,8 +704,17 @@
       <c r="J6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="4:10" ht="17.399999999999999">
+    <row r="7" spans="4:13" ht="17.399999999999999">
       <c r="D7" s="5" t="s">
         <v>2</v>
       </c>
@@ -689,8 +736,17 @@
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="4:10" ht="17.399999999999999">
+    <row r="8" spans="4:13" ht="17.399999999999999">
       <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
@@ -712,8 +768,17 @@
       <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="4:10" ht="17.399999999999999">
+    <row r="9" spans="4:13" ht="17.399999999999999">
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
@@ -735,8 +800,17 @@
       <c r="J9" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="10" spans="4:10" ht="17.399999999999999">
+    <row r="10" spans="4:13" ht="17.399999999999999">
       <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
@@ -758,8 +832,17 @@
       <c r="J10" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" spans="4:10" ht="17.399999999999999">
+    <row r="11" spans="4:13" ht="17.399999999999999">
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
@@ -781,8 +864,17 @@
       <c r="J11" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="4:10" ht="17.399999999999999">
+    <row r="12" spans="4:13" ht="17.399999999999999">
       <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
@@ -804,14 +896,25 @@
       <c r="J12" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
>> update 20241018 result
.
</commit_message>
<xml_diff>
--- a/chatgpt_performance_metric/Evaluation_Release_Result/Evaluation_Release_History.xlsx
+++ b/chatgpt_performance_metric/Evaluation_Release_Result/Evaluation_Release_History.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\project\AI_Application\rag\source\ragas_evaluation\perf_metric\chatgpt_performance_metric\evaluation_release_result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\tom\python_project\Testset_Generation_Evaluation\perf_metric\chatgpt_performance_metric\Evaluation_Release_Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A46EBAB-E4FD-4454-B7CC-95DBB792A9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679C819B-3D0E-408E-8E02-C944FE86939A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85E0B42A-1E2E-4653-9973-9AFC057EC341}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{85E0B42A-1E2E-4653-9973-9AFC057EC341}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Release_History" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
   <si>
     <t>challenger.txt</t>
   </si>
@@ -84,10 +84,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TBD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Getting Started 20240923.docx (Device Farm)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,6 +96,12 @@
     <t>contexts,
 answer
 * 어떤 Vertorization 환경에서 추출한건가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>embedding &amp;
+vectorization
+(별도(??). Server - CSV 적용)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -111,14 +113,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="맑은 고딕"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -138,7 +140,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,12 +156,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,44 +208,35 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="58" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -586,22 +573,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D663431-DE91-43EB-971D-8A92CF748157}">
-  <dimension ref="D3:M12"/>
+  <dimension ref="D3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="8.8984375" style="1"/>
-    <col min="4" max="4" width="57.3984375" style="1" customWidth="1"/>
-    <col min="5" max="133" width="15.796875" style="1" customWidth="1"/>
-    <col min="134" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="57.44140625" style="1" customWidth="1"/>
+    <col min="5" max="130" width="15.77734375" style="1" customWidth="1"/>
+    <col min="131" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:13" ht="17.399999999999999">
-      <c r="D3" s="9" t="s">
+    <row r="3" spans="4:10" ht="17.399999999999999">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="7">
@@ -609,309 +596,222 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="8">
-        <v>45553</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="10">
+      <c r="H3" s="9">
         <v>45583</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="4:13" ht="87">
-      <c r="D4" s="9"/>
-      <c r="E4" s="3" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="4:10" ht="104.4">
+      <c r="D4" s="8"/>
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="4:13" ht="17.399999999999999">
-      <c r="D5" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" ht="17.399999999999999">
+      <c r="D5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" ht="17.399999999999999">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" ht="17.399999999999999">
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" ht="17.399999999999999">
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" ht="17.399999999999999">
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" ht="17.399999999999999">
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" ht="17.399999999999999">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="4:13" ht="17.399999999999999">
-      <c r="D6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="4:13" ht="17.399999999999999">
-      <c r="D7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="4:13" ht="17.399999999999999">
-      <c r="D8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="4:13" ht="17.399999999999999">
-      <c r="D9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="4:13" ht="17.399999999999999">
-      <c r="D10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="4:13" ht="17.399999999999999">
-      <c r="D11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="4:13" ht="17.399999999999999">
-      <c r="D12" s="5" t="s">
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" ht="17.399999999999999">
+      <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="12" t="s">
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="H3:J3"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>